<commit_message>
Update in CLick event
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_Sanity\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA42168-8997-4068-9B55-FC88720F39B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4256E4E3-138E-473A-847A-256EC9A3F9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
   <si>
     <t>TestCase</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>WAIT</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -618,30 +621,24 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
@@ -649,43 +646,43 @@
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -694,13 +691,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -709,27 +706,29 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
@@ -737,7 +736,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
@@ -750,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>35</v>
@@ -763,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>35</v>
@@ -773,30 +772,30 @@
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
@@ -804,12 +803,25 @@
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1112,18 +1124,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1146,18 +1158,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update in CLick event11
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4256E4E3-138E-473A-847A-256EC9A3F9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98EBB0B-9929-4BBF-A59D-DD9D726B2979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>TestCase</t>
   </si>
@@ -205,12 +205,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -560,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -606,98 +605,92 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>17</v>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
+      <c r="E8" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -706,13 +699,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -721,35 +714,37 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
-        <v>9</v>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>35</v>
@@ -758,11 +753,11 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>35</v>
@@ -771,11 +766,11 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>
@@ -784,44 +779,57 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
-        <v>32</v>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
-      <c r="B17" s="5" t="s">
-        <v>9</v>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -861,7 +869,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -869,7 +877,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -880,7 +888,7 @@
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -888,7 +896,7 @@
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -896,7 +904,7 @@
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1124,18 +1132,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1158,18 +1166,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update in CLick event12
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98EBB0B-9929-4BBF-A59D-DD9D726B2979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7720B637-66C7-4E5E-8F88-CDFC06D549CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>TestCase</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -754,14 +754,10 @@
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
@@ -770,7 +766,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>
@@ -780,42 +776,32 @@
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
@@ -824,12 +810,53 @@
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
Update in CLick event13
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7720B637-66C7-4E5E-8F88-CDFC06D549CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8469DBC4-30A9-4CFC-8AC1-CC7ADF90B51B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>TestCase</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>WAIT</t>
+  </si>
+  <si>
+    <t>SCROLL_DOWN</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -754,7 +757,7 @@
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -763,87 +766,83 @@
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
@@ -851,12 +850,25 @@
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
Update in CLick event14
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8469DBC4-30A9-4CFC-8AC1-CC7ADF90B51B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F6D057-D3D2-4B95-A84C-1BA50FEB3925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>TestCase</t>
   </si>
@@ -89,15 +89,6 @@
     <t>RegistrationZip</t>
   </si>
   <si>
-    <t>ExistingaccNObutton</t>
-  </si>
-  <si>
-    <t>T&amp;CCHeckbox</t>
-  </si>
-  <si>
-    <t>RegistrationSubmit</t>
-  </si>
-  <si>
     <t>RegistrationSuccessMSG</t>
   </si>
   <si>
@@ -119,22 +110,13 @@
     <t>auto</t>
   </si>
   <si>
-    <t>VERIFY_TEXT_PRESENT</t>
-  </si>
-  <si>
     <t>$BaseURL</t>
   </si>
   <si>
-    <t>Acctype</t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
     <t>WAIT</t>
-  </si>
-  <si>
-    <t>SCROLL_DOWN</t>
   </si>
 </sst>
 </file>
@@ -562,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -610,7 +592,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -625,14 +607,14 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -647,7 +629,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -660,7 +642,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>16</v>
@@ -675,7 +657,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>17</v>
@@ -684,13 +666,13 @@
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
@@ -705,7 +687,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
@@ -720,7 +702,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
@@ -735,7 +717,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>21</v>
@@ -747,128 +729,25 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -904,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -912,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -920,7 +799,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -928,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -936,7 +815,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -944,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -957,10 +836,10 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1171,18 +1050,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1205,18 +1084,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update in CLick event15
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F6D057-D3D2-4B95-A84C-1BA50FEB3925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA42ACC-4B83-4A77-A593-7A38C4A8B7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>TestCase</t>
   </si>
@@ -59,12 +59,6 @@
     <t>ENTERTEXT</t>
   </si>
   <si>
-    <t>MyaccountSection</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>TC23_Verify_UserRegistration</t>
   </si>
   <si>
@@ -89,6 +83,9 @@
     <t>RegistrationZip</t>
   </si>
   <si>
+    <t>ExistingaccNObutton</t>
+  </si>
+  <si>
     <t>RegistrationSuccessMSG</t>
   </si>
   <si>
@@ -113,10 +110,16 @@
     <t>$BaseURL</t>
   </si>
   <si>
+    <t>Acctype</t>
+  </si>
+  <si>
     <t>CSS</t>
   </si>
   <si>
     <t>WAIT</t>
+  </si>
+  <si>
+    <t>SCROLL_DOWN</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -578,7 +581,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -626,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
@@ -639,13 +642,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -654,28 +657,28 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -684,13 +687,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -699,13 +702,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -714,13 +717,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -729,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>30</v>
@@ -739,15 +742,33 @@
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -783,52 +804,52 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3">
         <v>75230</v>
@@ -836,10 +857,10 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes done for Javascriptexecutor elements
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA42ACC-4B83-4A77-A593-7A38C4A8B7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B6926-4D32-4D57-9F43-56174CA95A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
   <si>
     <t>TestCase</t>
   </si>
@@ -83,43 +83,91 @@
     <t>RegistrationZip</t>
   </si>
   <si>
+    <t>RegistrationSuccessMSG</t>
+  </si>
+  <si>
+    <t>ENTER_RANDOM_VALUE</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Autest@automation.com</t>
+  </si>
+  <si>
+    <t>Test@1234</t>
+  </si>
+  <si>
+    <t>$BaseURL</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
+    <t>SCROLL_DOWN</t>
+  </si>
+  <si>
+    <t>CLICK_PRE_ENTERTEXT</t>
+  </si>
+  <si>
+    <t>T&amp;CCHeckbox</t>
+  </si>
+  <si>
+    <t>RegistrationSubmit</t>
+  </si>
+  <si>
+    <t>VERIFY_TEXT_PRESENT</t>
+  </si>
+  <si>
+    <t>MyaccountSection</t>
+  </si>
+  <si>
+    <t>Acctype</t>
+  </si>
+  <si>
     <t>ExistingaccNObutton</t>
   </si>
   <si>
-    <t>RegistrationSuccessMSG</t>
-  </si>
-  <si>
-    <t>ENTER_RANDOM_VALUE</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Autest@automation.com</t>
-  </si>
-  <si>
-    <t>Test@1234</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>$BaseURL</t>
-  </si>
-  <si>
-    <t>Acctype</t>
-  </si>
-  <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>WAIT</t>
-  </si>
-  <si>
-    <t>SCROLL_DOWN</t>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>CLICK_JS</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>RadioButton</t>
+  </si>
+  <si>
+    <t>Elementype1</t>
+  </si>
+  <si>
+    <t>Elementype2</t>
+  </si>
+  <si>
+    <t>Elementype3</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Elementype4</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -547,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -595,7 +643,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -610,29 +658,33 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -645,7 +697,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>14</v>
@@ -653,96 +705,92 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -751,38 +799,209 @@
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -804,7 +1023,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -812,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -820,7 +1039,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -828,7 +1047,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -836,7 +1055,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -844,7 +1063,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -857,10 +1076,42 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabling User registration testcase with additional waits
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B6926-4D32-4D57-9F43-56174CA95A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01752A1-8485-44DD-85D0-C3ECA9CE1E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>TestCase</t>
   </si>
@@ -595,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -951,30 +951,26 @@
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
@@ -982,12 +978,25 @@
         <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1001,7 +1010,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1125,6 +1134,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1321,15 +1339,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1337,6 +1346,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1355,14 +1372,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Functional change in TC23
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01752A1-8485-44DD-85D0-C3ECA9CE1E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8146F5F6-4A83-4DFA-8AE7-2A5ACA04D97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
   <si>
     <t>TestCase</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Profile</t>
+  </si>
+  <si>
+    <t>Elementype5</t>
+  </si>
+  <si>
+    <t>PromoCheckbox</t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -906,13 +912,13 @@
         <v>39</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -930,13 +936,13 @@
         <v>39</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -951,52 +957,76 @@
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1007,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1123,6 +1153,14 @@
         <v>47</v>
       </c>
     </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{56619A5F-EADA-4190-AFA5-B6FA50B984EC}"/>
@@ -1134,12 +1172,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1340,15 +1375,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1373,10 +1412,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOM Change on ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8146F5F6-4A83-4DFA-8AE7-2A5ACA04D97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0581AFF-4FC8-4423-815C-723066180ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>TestCase</t>
   </si>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -990,43 +990,61 @@
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1178,6 +1196,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1374,15 +1401,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
@@ -1393,6 +1411,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1409,12 +1435,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>